<commit_message>
Cypher query conversion done!!
</commit_message>
<xml_diff>
--- a/qa/QA.xlsx
+++ b/qa/QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\PES_SEM_8\KGraphs-QA\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8108FDA3-B3F8-46BE-9EFD-77E20A52AAB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B05243-846C-4C03-9961-995314A19391}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Question-Intent" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+  <si>
+    <t>Manually map</t>
+  </si>
+  <si>
+    <t>TrNAP - TrWP</t>
+  </si>
+  <si>
+    <t>TrAP - TrIP</t>
+  </si>
+  <si>
+    <t>TeCP -&gt; TeRP</t>
+  </si>
   <si>
     <t>Intent</t>
   </si>
@@ -30,34 +42,18 @@
     <t>Query</t>
   </si>
   <si>
+    <t>disease_symptom</t>
+  </si>
+  <si>
     <t>Slno</t>
   </si>
   <si>
-    <t>Manually map</t>
-  </si>
-  <si>
-    <t>TrNAP - TrWP</t>
-  </si>
-  <si>
     <t>Question</t>
   </si>
   <si>
-    <t>TrAP - TrIP</t>
-  </si>
-  <si>
-    <t>TeCP -&gt; TeRP</t>
-  </si>
-  <si>
-    <t>disease_symptom</t>
-  </si>
-  <si>
     <t>Relation</t>
   </si>
   <si>
-    <t>MATCH (Problem {name:"disease_name"})-[:has_symptom]-(y)
-RETURN Problem , y</t>
-  </si>
-  <si>
     <t>what are symptoms of Problem</t>
   </si>
   <si>
@@ -85,15 +81,30 @@
     <t>disease_treatment</t>
   </si>
   <si>
+    <t>MATCH (x)-[:has_symptom]-(Symptom)
+WHERE Symptom.name =~ '(?i).*entity_name.*'
+RETURN Symptom, x</t>
+  </si>
+  <si>
     <t>TrIP</t>
   </si>
   <si>
     <t>what diseases are cured by treatment</t>
   </si>
   <si>
+    <t>MATCH (Treatment)-[:treatment_caused]-(x)
+WHERE Treatment.name =~ '(?i).*entity_name.*'
+RETURN Treatment, x</t>
+  </si>
+  <si>
     <t>treatment_disease</t>
   </si>
   <si>
+    <t>MATCH (x)-[:treats_disease]-(Problem)
+WHERE Problem.name =~ '(?i).*entity_name.*'
+RETURN Problem, x</t>
+  </si>
+  <si>
     <t xml:space="preserve"> what problem is a test conducted for</t>
   </si>
   <si>
@@ -103,17 +114,28 @@
     <t>TeRP</t>
   </si>
   <si>
+    <t>MATCH (Treatment)-[:treats_disease]-(x)
+WHERE Treatment.name =~ '(?i).*treatment_name.*'
+RETURN Treatment, x</t>
+  </si>
+  <si>
     <t>what tests are conducted for Problem</t>
   </si>
   <si>
     <t>problem_test</t>
   </si>
   <si>
+    <t>MATCH (Test)-[:indicates_disease]-(x)
+WHERE Test.name =~ '(?i).*entity_name.*'
+RETURN Test, x</t>
+  </si>
+  <si>
     <t>What are the signs that I have Problem?</t>
   </si>
   <si>
-    <t>MATCH (x)-[:has_symptom]-(Symptom{name:"symptom_name"})
-RETURN Symptom, x</t>
+    <t>MATCH (x)-[:indicates_disease]-(Problem)
+WHERE Problem.name =~ '(?i).*entity_name.*'
+RETURN Problem, x</t>
   </si>
   <si>
     <t>is problem a symptom of problem</t>
@@ -125,10 +147,6 @@
     <t>I have problem, what treatment do I take?</t>
   </si>
   <si>
-    <t>MATCH (Treatment{name:"treatment_name"})-[:treatment_caused]-(x)
-RETURN Treatment, x</t>
-  </si>
-  <si>
     <t xml:space="preserve">is treatment helpful for problem? </t>
   </si>
   <si>
@@ -141,10 +159,6 @@
     <t>Can treatment cause problem?</t>
   </si>
   <si>
-    <t>MATCH (x)-[:treats_disease]-(Problem{name: "disease_name"})
-RETURN Problem, x</t>
-  </si>
-  <si>
     <t>I am suffering from problem. does treatment cure it?</t>
   </si>
   <si>
@@ -154,22 +168,18 @@
     <t xml:space="preserve">My doctor told me I experience problem. Do I have problem? </t>
   </si>
   <si>
-    <t>MATCH (Treatment{name: "treatment_name"})-[:treats_disease]-(x)
-RETURN Treatment, x</t>
-  </si>
-  <si>
-    <t>MATCH (Test{name:"test_name"})-[:indicates_disease]-(x)
-RETURN Test, x</t>
-  </si>
-  <si>
-    <t>MATCH (x)-[:indicates_disease]-(Problem{name: "disease_name"})
-RETURN Problem, x</t>
-  </si>
-  <si>
     <t>I have problem. Is medicine the correct treatment?</t>
   </si>
   <si>
     <t>What all problems does a test reveal?</t>
+  </si>
+  <si>
+    <t>MATCH (Problem)-[:has_symptom]-(x)
+WHERE Problem.name =~ '(?i).*entity_name.*'
+RETURN Problem , x</t>
+  </si>
+  <si>
+    <t>treatment_side-effects</t>
   </si>
 </sst>
 </file>
@@ -544,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -560,13 +570,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -577,13 +587,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -591,13 +601,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -605,13 +615,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -619,10 +629,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -636,7 +646,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -647,13 +657,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -661,13 +671,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -675,13 +685,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -689,13 +699,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -703,13 +713,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -717,10 +727,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -731,10 +741,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -745,13 +755,13 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -759,13 +769,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -773,13 +783,13 @@
         <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
         <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -787,10 +797,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -801,10 +811,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -815,13 +825,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
@@ -829,13 +839,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
@@ -843,27 +853,27 @@
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1"/>
@@ -1854,7 +1864,9 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1864,66 +1876,66 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1931,6 +1943,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1947,22 +1960,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>